<commit_message>
Before removing navigation props
</commit_message>
<xml_diff>
--- a/szakdolgozat/szakdolgozat-idobeosztas.xlsx
+++ b/szakdolgozat/szakdolgozat-idobeosztas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\torok\source\repos\szakdolgozat\szakdolgozat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E80DF150-D5B9-495B-B037-CB87F50A5AE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1BF1AD-18D5-4A9A-B193-F677DAE6992F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DDD22623-F967-449E-AB02-C266B1977814}"/>
+    <workbookView xWindow="-40" yWindow="-40" windowWidth="19280" windowHeight="10160" xr2:uid="{DDD22623-F967-449E-AB02-C266B1977814}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -95,7 +95,7 @@
     <t>Máj</t>
   </si>
   <si>
-    <t>Jún</t>
+    <t>Admin felület a rendelések kezelésére</t>
   </si>
 </sst>
 </file>
@@ -241,15 +241,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="4" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="4" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -570,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{006FF946-6410-4AC6-BB3F-75DF2F6E6EBB}">
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,58 +581,54 @@
     <col min="1" max="1" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
-      <c r="B1" s="6">
+      <c r="B1" s="9">
         <v>2023</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6">
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9">
         <v>2024</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-    </row>
-    <row r="2" spans="1:11" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8" t="s">
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+    </row>
+    <row r="2" spans="1:10" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="6"/>
+      <c r="B2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+    </row>
+    <row r="3" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="3"/>
@@ -644,10 +640,9 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="2"/>
@@ -659,10 +654,9 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+    </row>
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="2"/>
@@ -674,40 +668,37 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>4</v>
+    </row>
+    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>3</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="F6" s="4"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>3</v>
+    </row>
+    <row r="7" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>4</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="4"/>
+      <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+    </row>
+    <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
@@ -715,14 +706,13 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+    </row>
+    <row r="9" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="2"/>
@@ -731,13 +721,12 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+    </row>
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="2"/>
@@ -746,14 +735,13 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="2"/>
       <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>7</v>
+    </row>
+    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -761,14 +749,13 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>9</v>
+      <c r="H11" s="3"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -776,21 +763,31 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H12" s="3"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
@@ -867,11 +864,14 @@
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="F1:J1"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>